<commit_message>
yeni dosya sisteminde ilk değişiklik
</commit_message>
<xml_diff>
--- a/süre yönetimi.xlsx
+++ b/süre yönetimi.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>süre önemlidir</t>
+  </si>
+  <si>
+    <t>süre bitti</t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3"/>
+  <dimension ref="B3:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -362,6 +365,11 @@
     <row r="3" spans="2:2">
       <c r="B3" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>